<commit_message>
Fixes to several Excel match logs
</commit_message>
<xml_diff>
--- a/source/excel/nwsl-2016-bos-wnyf-090716.xlsx
+++ b/source/excel/nwsl-2016-bos-wnyf-090716.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/Desktop/push/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/Documents/GitHub/wosostats/source/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EE4A4D-3235-734C-94FD-11E47C106E9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="7440" windowWidth="20140" windowHeight="8560" tabRatio="500"/>
+    <workbookView xWindow="5020" yWindow="1120" windowWidth="20140" windowHeight="11220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,10 +18,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$1430</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -752,7 +761,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1011,6 +1020,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1278,13 +1290,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A984" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="G112" sqref="G112"/>
+      <selection pane="bottomLeft" activeCell="E998" sqref="E998"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -56437,7 +56449,7 @@
         <v>226</v>
       </c>
       <c r="F997" s="25" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="G997" s="25"/>
       <c r="H997" s="25"/>
@@ -72086,17 +72098,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I8" r:id="rId1"/>
-    <hyperlink ref="F23" r:id="rId2"/>
-    <hyperlink ref="F28" r:id="rId3"/>
-    <hyperlink ref="F29" r:id="rId4"/>
-    <hyperlink ref="I107" r:id="rId5"/>
-    <hyperlink ref="I149" r:id="rId6"/>
-    <hyperlink ref="I155" r:id="rId7"/>
-    <hyperlink ref="I234" r:id="rId8"/>
-    <hyperlink ref="I279" r:id="rId9"/>
-    <hyperlink ref="I378" r:id="rId10"/>
-    <hyperlink ref="I596" r:id="rId11"/>
+    <hyperlink ref="I8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F23" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F28" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F29" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="I107" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="I149" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="I155" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="I234" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="I279" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="I378" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="I596" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>